<commit_message>
removed img and .png
</commit_message>
<xml_diff>
--- a/AuraSkypoolDXB/Result.xlsx
+++ b/AuraSkypoolDXB/Result.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img1.png</t>
+          <t>AuraSkypoolDXB-1</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -506,7 +506,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img2.png</t>
+          <t>AuraSkypoolDXB-2</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -536,7 +536,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img3.png</t>
+          <t>AuraSkypoolDXB-3</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img4.png</t>
+          <t>AuraSkypoolDXB-4</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -596,7 +596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img5.png</t>
+          <t>AuraSkypoolDXB-5</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -626,7 +626,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img6.png</t>
+          <t>AuraSkypoolDXB-6</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -656,7 +656,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img7.png</t>
+          <t>AuraSkypoolDXB-7</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -686,7 +686,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img8.png</t>
+          <t>AuraSkypoolDXB-8</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -716,7 +716,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img9.png</t>
+          <t>AuraSkypoolDXB-9</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -746,7 +746,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img10.png</t>
+          <t>AuraSkypoolDXB-10</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img11.png</t>
+          <t>AuraSkypoolDXB-11</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -806,7 +806,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img12.png</t>
+          <t>AuraSkypoolDXB-12</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -836,7 +836,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img13.png</t>
+          <t>AuraSkypoolDXB-13</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -866,7 +866,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img14.png</t>
+          <t>AuraSkypoolDXB-14</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -896,7 +896,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img15.png</t>
+          <t>AuraSkypoolDXB-15</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -926,7 +926,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img16.png</t>
+          <t>AuraSkypoolDXB-16</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -956,7 +956,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img17.png</t>
+          <t>AuraSkypoolDXB-17</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -986,7 +986,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img18.png</t>
+          <t>AuraSkypoolDXB-18</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img19.png</t>
+          <t>AuraSkypoolDXB-19</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img20.png</t>
+          <t>AuraSkypoolDXB-20</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img21.png</t>
+          <t>AuraSkypoolDXB-21</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img22.png</t>
+          <t>AuraSkypoolDXB-22</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img23.png</t>
+          <t>AuraSkypoolDXB-23</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img24.png</t>
+          <t>AuraSkypoolDXB-24</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img25.png</t>
+          <t>AuraSkypoolDXB-25</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img26.png</t>
+          <t>AuraSkypoolDXB-26</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img27.png</t>
+          <t>AuraSkypoolDXB-27</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img28.png</t>
+          <t>AuraSkypoolDXB-28</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1316,7 +1316,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img29.png</t>
+          <t>AuraSkypoolDXB-29</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img30.png</t>
+          <t>AuraSkypoolDXB-30</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img31.png</t>
+          <t>AuraSkypoolDXB-31</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img32.png</t>
+          <t>AuraSkypoolDXB-32</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img33.png</t>
+          <t>AuraSkypoolDXB-33</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1466,7 +1466,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img34.png</t>
+          <t>AuraSkypoolDXB-34</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img35.png</t>
+          <t>AuraSkypoolDXB-35</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img36.png</t>
+          <t>AuraSkypoolDXB-36</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img37.png</t>
+          <t>AuraSkypoolDXB-37</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img38.png</t>
+          <t>AuraSkypoolDXB-38</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img39.png</t>
+          <t>AuraSkypoolDXB-39</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img40.png</t>
+          <t>AuraSkypoolDXB-40</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1676,7 +1676,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img41.png</t>
+          <t>AuraSkypoolDXB-41</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1706,7 +1706,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img42.png</t>
+          <t>AuraSkypoolDXB-42</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1736,7 +1736,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img43.png</t>
+          <t>AuraSkypoolDXB-43</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img44.png</t>
+          <t>AuraSkypoolDXB-44</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img45.png</t>
+          <t>AuraSkypoolDXB-45</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1826,7 +1826,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img46.png</t>
+          <t>AuraSkypoolDXB-46</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img47.png</t>
+          <t>AuraSkypoolDXB-47</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1886,7 +1886,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img48.png</t>
+          <t>AuraSkypoolDXB-48</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1916,7 +1916,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img49.png</t>
+          <t>AuraSkypoolDXB-49</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img50.png</t>
+          <t>AuraSkypoolDXB-50</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img51.png</t>
+          <t>AuraSkypoolDXB-51</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img52.png</t>
+          <t>AuraSkypoolDXB-52</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -2036,7 +2036,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img53.png</t>
+          <t>AuraSkypoolDXB-53</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -2066,7 +2066,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img54.png</t>
+          <t>AuraSkypoolDXB-54</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -2096,7 +2096,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img55.png</t>
+          <t>AuraSkypoolDXB-55</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img56.png</t>
+          <t>AuraSkypoolDXB-56</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -2156,7 +2156,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img57.png</t>
+          <t>AuraSkypoolDXB-57</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -2186,7 +2186,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img58.png</t>
+          <t>AuraSkypoolDXB-58</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img59.png</t>
+          <t>AuraSkypoolDXB-59</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -2246,7 +2246,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img60.png</t>
+          <t>AuraSkypoolDXB-60</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -2276,7 +2276,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img61.png</t>
+          <t>AuraSkypoolDXB-61</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img62.png</t>
+          <t>AuraSkypoolDXB-62</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img63.png</t>
+          <t>AuraSkypoolDXB-63</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -2366,7 +2366,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img64.png</t>
+          <t>AuraSkypoolDXB-64</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -2396,7 +2396,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img65.png</t>
+          <t>AuraSkypoolDXB-65</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img66.png</t>
+          <t>AuraSkypoolDXB-66</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -2456,7 +2456,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img67.png</t>
+          <t>AuraSkypoolDXB-67</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img68.png</t>
+          <t>AuraSkypoolDXB-68</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -2516,7 +2516,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img69.png</t>
+          <t>AuraSkypoolDXB-69</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -2546,7 +2546,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img70.png</t>
+          <t>AuraSkypoolDXB-70</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -2576,7 +2576,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img71.png</t>
+          <t>AuraSkypoolDXB-71</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img72.png</t>
+          <t>AuraSkypoolDXB-72</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -2636,7 +2636,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img73.png</t>
+          <t>AuraSkypoolDXB-73</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -2666,7 +2666,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img74.png</t>
+          <t>AuraSkypoolDXB-74</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -2696,7 +2696,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img75.png</t>
+          <t>AuraSkypoolDXB-75</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img76.png</t>
+          <t>AuraSkypoolDXB-76</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -2756,7 +2756,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img77.png</t>
+          <t>AuraSkypoolDXB-77</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -2786,7 +2786,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img78.png</t>
+          <t>AuraSkypoolDXB-78</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -2816,7 +2816,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img79.png</t>
+          <t>AuraSkypoolDXB-79</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -2846,7 +2846,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img80.png</t>
+          <t>AuraSkypoolDXB-80</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img81.png</t>
+          <t>AuraSkypoolDXB-81</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -2906,7 +2906,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img82.png</t>
+          <t>AuraSkypoolDXB-82</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -2936,7 +2936,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img83.png</t>
+          <t>AuraSkypoolDXB-83</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -2966,7 +2966,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img84.png</t>
+          <t>AuraSkypoolDXB-84</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -2996,7 +2996,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img85.png</t>
+          <t>AuraSkypoolDXB-85</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -3026,7 +3026,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img86.png</t>
+          <t>AuraSkypoolDXB-86</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -3056,7 +3056,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img87.png</t>
+          <t>AuraSkypoolDXB-87</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -3086,7 +3086,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img88.png</t>
+          <t>AuraSkypoolDXB-88</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -3116,7 +3116,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img89.png</t>
+          <t>AuraSkypoolDXB-89</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -3146,7 +3146,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img90.png</t>
+          <t>AuraSkypoolDXB-90</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -3176,7 +3176,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img91.png</t>
+          <t>AuraSkypoolDXB-91</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img92.png</t>
+          <t>AuraSkypoolDXB-92</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -3236,7 +3236,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img93.png</t>
+          <t>AuraSkypoolDXB-93</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -3266,7 +3266,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img94.png</t>
+          <t>AuraSkypoolDXB-94</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -3296,7 +3296,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img95.png</t>
+          <t>AuraSkypoolDXB-95</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -3326,7 +3326,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img96.png</t>
+          <t>AuraSkypoolDXB-96</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -3356,7 +3356,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img97.png</t>
+          <t>AuraSkypoolDXB-97</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -3386,7 +3386,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img98.png</t>
+          <t>AuraSkypoolDXB-98</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -3416,7 +3416,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img99.png</t>
+          <t>AuraSkypoolDXB-99</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -3446,7 +3446,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img100.png</t>
+          <t>AuraSkypoolDXB-100</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -3476,7 +3476,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img101.png</t>
+          <t>AuraSkypoolDXB-101</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -3506,7 +3506,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img102.png</t>
+          <t>AuraSkypoolDXB-102</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -3536,7 +3536,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img103.png</t>
+          <t>AuraSkypoolDXB-103</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -3566,7 +3566,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img104.png</t>
+          <t>AuraSkypoolDXB-104</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -3596,7 +3596,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img105.png</t>
+          <t>AuraSkypoolDXB-105</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -3626,7 +3626,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img106.png</t>
+          <t>AuraSkypoolDXB-106</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -3656,7 +3656,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img107.png</t>
+          <t>AuraSkypoolDXB-107</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -3686,7 +3686,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img108.png</t>
+          <t>AuraSkypoolDXB-108</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -3716,7 +3716,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img109.png</t>
+          <t>AuraSkypoolDXB-109</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -3746,7 +3746,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img110.png</t>
+          <t>AuraSkypoolDXB-110</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -3776,7 +3776,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img111.png</t>
+          <t>AuraSkypoolDXB-111</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -3806,7 +3806,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img112.png</t>
+          <t>AuraSkypoolDXB-112</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -3836,7 +3836,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img113.png</t>
+          <t>AuraSkypoolDXB-113</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img114.png</t>
+          <t>AuraSkypoolDXB-114</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -3896,7 +3896,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img115.png</t>
+          <t>AuraSkypoolDXB-115</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -3926,7 +3926,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img116.png</t>
+          <t>AuraSkypoolDXB-116</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -3956,7 +3956,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img117.png</t>
+          <t>AuraSkypoolDXB-117</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -3986,7 +3986,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img118.png</t>
+          <t>AuraSkypoolDXB-118</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -4016,7 +4016,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img119.png</t>
+          <t>AuraSkypoolDXB-119</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -4046,7 +4046,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img120.png</t>
+          <t>AuraSkypoolDXB-120</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -4076,7 +4076,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img121.png</t>
+          <t>AuraSkypoolDXB-121</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img122.png</t>
+          <t>AuraSkypoolDXB-122</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -4136,7 +4136,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img123.png</t>
+          <t>AuraSkypoolDXB-123</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -4166,7 +4166,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img124.png</t>
+          <t>AuraSkypoolDXB-124</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -4196,7 +4196,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img125.png</t>
+          <t>AuraSkypoolDXB-125</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -4226,7 +4226,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img126.png</t>
+          <t>AuraSkypoolDXB-126</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -4256,7 +4256,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img127.png</t>
+          <t>AuraSkypoolDXB-127</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -4286,7 +4286,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img128.png</t>
+          <t>AuraSkypoolDXB-128</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -4316,7 +4316,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img129.png</t>
+          <t>AuraSkypoolDXB-129</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -4346,7 +4346,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img130.png</t>
+          <t>AuraSkypoolDXB-130</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -4376,7 +4376,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img131.png</t>
+          <t>AuraSkypoolDXB-131</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -4406,7 +4406,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img132.png</t>
+          <t>AuraSkypoolDXB-132</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -4436,7 +4436,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img133.png</t>
+          <t>AuraSkypoolDXB-133</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -4466,7 +4466,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img134.png</t>
+          <t>AuraSkypoolDXB-134</t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -4496,7 +4496,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img135.png</t>
+          <t>AuraSkypoolDXB-135</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -4526,7 +4526,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img136.png</t>
+          <t>AuraSkypoolDXB-136</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -4556,7 +4556,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img137.png</t>
+          <t>AuraSkypoolDXB-137</t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -4586,7 +4586,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img138.png</t>
+          <t>AuraSkypoolDXB-138</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -4616,7 +4616,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img139.png</t>
+          <t>AuraSkypoolDXB-139</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -4646,7 +4646,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img140.png</t>
+          <t>AuraSkypoolDXB-140</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -4676,7 +4676,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img141.png</t>
+          <t>AuraSkypoolDXB-141</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -4706,7 +4706,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img142.png</t>
+          <t>AuraSkypoolDXB-142</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -4736,7 +4736,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img143.png</t>
+          <t>AuraSkypoolDXB-143</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img144.png</t>
+          <t>AuraSkypoolDXB-144</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -4796,7 +4796,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img145.png</t>
+          <t>AuraSkypoolDXB-145</t>
         </is>
       </c>
       <c r="C146" t="n">
@@ -4826,7 +4826,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img146.png</t>
+          <t>AuraSkypoolDXB-146</t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -4856,7 +4856,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img147.png</t>
+          <t>AuraSkypoolDXB-147</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -4886,7 +4886,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img148.png</t>
+          <t>AuraSkypoolDXB-148</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -4916,7 +4916,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img149.png</t>
+          <t>AuraSkypoolDXB-149</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -4946,7 +4946,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img150.png</t>
+          <t>AuraSkypoolDXB-150</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -4976,7 +4976,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img151.png</t>
+          <t>AuraSkypoolDXB-151</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -5006,7 +5006,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img152.png</t>
+          <t>AuraSkypoolDXB-152</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -5036,7 +5036,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img153.png</t>
+          <t>AuraSkypoolDXB-153</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -5066,7 +5066,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img154.png</t>
+          <t>AuraSkypoolDXB-154</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -5096,7 +5096,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img155.png</t>
+          <t>AuraSkypoolDXB-155</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -5126,7 +5126,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img156.png</t>
+          <t>AuraSkypoolDXB-156</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -5156,7 +5156,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img157.png</t>
+          <t>AuraSkypoolDXB-157</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -5186,7 +5186,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img158.png</t>
+          <t>AuraSkypoolDXB-158</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -5216,7 +5216,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img159.png</t>
+          <t>AuraSkypoolDXB-159</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -5246,7 +5246,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img160.png</t>
+          <t>AuraSkypoolDXB-160</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -5276,7 +5276,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img161.png</t>
+          <t>AuraSkypoolDXB-161</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -5306,7 +5306,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img162.png</t>
+          <t>AuraSkypoolDXB-162</t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -5336,7 +5336,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img163.png</t>
+          <t>AuraSkypoolDXB-163</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -5366,7 +5366,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img164.png</t>
+          <t>AuraSkypoolDXB-164</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -5396,7 +5396,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img165.png</t>
+          <t>AuraSkypoolDXB-165</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -5426,7 +5426,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img166.png</t>
+          <t>AuraSkypoolDXB-166</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -5456,7 +5456,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img167.png</t>
+          <t>AuraSkypoolDXB-167</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -5486,7 +5486,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img168.png</t>
+          <t>AuraSkypoolDXB-168</t>
         </is>
       </c>
       <c r="C169" t="n">
@@ -5516,7 +5516,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img169.png</t>
+          <t>AuraSkypoolDXB-169</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -5546,7 +5546,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img170.png</t>
+          <t>AuraSkypoolDXB-170</t>
         </is>
       </c>
       <c r="C171" t="n">
@@ -5576,7 +5576,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img171.png</t>
+          <t>AuraSkypoolDXB-171</t>
         </is>
       </c>
       <c r="C172" t="n">
@@ -5606,7 +5606,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img172.png</t>
+          <t>AuraSkypoolDXB-172</t>
         </is>
       </c>
       <c r="C173" t="n">
@@ -5636,7 +5636,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img173.png</t>
+          <t>AuraSkypoolDXB-173</t>
         </is>
       </c>
       <c r="C174" t="n">
@@ -5666,7 +5666,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img174.png</t>
+          <t>AuraSkypoolDXB-174</t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -5696,7 +5696,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img175.png</t>
+          <t>AuraSkypoolDXB-175</t>
         </is>
       </c>
       <c r="C176" t="n">
@@ -5726,7 +5726,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img176.png</t>
+          <t>AuraSkypoolDXB-176</t>
         </is>
       </c>
       <c r="C177" t="n">
@@ -5756,7 +5756,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img177.png</t>
+          <t>AuraSkypoolDXB-177</t>
         </is>
       </c>
       <c r="C178" t="n">
@@ -5786,7 +5786,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img178.png</t>
+          <t>AuraSkypoolDXB-178</t>
         </is>
       </c>
       <c r="C179" t="n">
@@ -5816,7 +5816,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img179.png</t>
+          <t>AuraSkypoolDXB-179</t>
         </is>
       </c>
       <c r="C180" t="n">
@@ -5846,7 +5846,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img180.png</t>
+          <t>AuraSkypoolDXB-180</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -5876,7 +5876,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img181.png</t>
+          <t>AuraSkypoolDXB-181</t>
         </is>
       </c>
       <c r="C182" t="n">
@@ -5906,7 +5906,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img182.png</t>
+          <t>AuraSkypoolDXB-182</t>
         </is>
       </c>
       <c r="C183" t="n">
@@ -5936,7 +5936,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img183.png</t>
+          <t>AuraSkypoolDXB-183</t>
         </is>
       </c>
       <c r="C184" t="n">
@@ -5966,7 +5966,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img184.png</t>
+          <t>AuraSkypoolDXB-184</t>
         </is>
       </c>
       <c r="C185" t="n">
@@ -5996,7 +5996,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img185.png</t>
+          <t>AuraSkypoolDXB-185</t>
         </is>
       </c>
       <c r="C186" t="n">
@@ -6026,7 +6026,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img186.png</t>
+          <t>AuraSkypoolDXB-186</t>
         </is>
       </c>
       <c r="C187" t="n">
@@ -6056,7 +6056,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img187.png</t>
+          <t>AuraSkypoolDXB-187</t>
         </is>
       </c>
       <c r="C188" t="n">
@@ -6086,7 +6086,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img188.png</t>
+          <t>AuraSkypoolDXB-188</t>
         </is>
       </c>
       <c r="C189" t="n">
@@ -6116,7 +6116,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img189.png</t>
+          <t>AuraSkypoolDXB-189</t>
         </is>
       </c>
       <c r="C190" t="n">
@@ -6146,7 +6146,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img190.png</t>
+          <t>AuraSkypoolDXB-190</t>
         </is>
       </c>
       <c r="C191" t="n">
@@ -6176,7 +6176,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img191.png</t>
+          <t>AuraSkypoolDXB-191</t>
         </is>
       </c>
       <c r="C192" t="n">
@@ -6206,7 +6206,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img192.png</t>
+          <t>AuraSkypoolDXB-192</t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -6236,7 +6236,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img193.png</t>
+          <t>AuraSkypoolDXB-193</t>
         </is>
       </c>
       <c r="C194" t="n">
@@ -6266,7 +6266,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img194.png</t>
+          <t>AuraSkypoolDXB-194</t>
         </is>
       </c>
       <c r="C195" t="n">
@@ -6296,7 +6296,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img195.png</t>
+          <t>AuraSkypoolDXB-195</t>
         </is>
       </c>
       <c r="C196" t="n">
@@ -6326,7 +6326,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img196.png</t>
+          <t>AuraSkypoolDXB-196</t>
         </is>
       </c>
       <c r="C197" t="n">
@@ -6356,7 +6356,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img197.png</t>
+          <t>AuraSkypoolDXB-197</t>
         </is>
       </c>
       <c r="C198" t="n">
@@ -6386,7 +6386,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img198.png</t>
+          <t>AuraSkypoolDXB-198</t>
         </is>
       </c>
       <c r="C199" t="n">
@@ -6416,7 +6416,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img199.png</t>
+          <t>AuraSkypoolDXB-199</t>
         </is>
       </c>
       <c r="C200" t="n">
@@ -6441,12 +6441,12 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>0x18404fe1e65f323a37963e8585d0e0fe488dde7c</t>
+          <t>0x3a4fdd7a51d388218a33b559a8c1a67f24791e6c</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img200.png</t>
+          <t>AuraSkypoolDXB-200</t>
         </is>
       </c>
       <c r="C201" t="n">
@@ -6476,7 +6476,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img201.png</t>
+          <t>AuraSkypoolDXB-201</t>
         </is>
       </c>
       <c r="C202" t="n">
@@ -6506,7 +6506,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img202.png</t>
+          <t>AuraSkypoolDXB-202</t>
         </is>
       </c>
       <c r="C203" t="n">
@@ -6536,7 +6536,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img203.png</t>
+          <t>AuraSkypoolDXB-203</t>
         </is>
       </c>
       <c r="C204" t="n">
@@ -6566,7 +6566,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img204.png</t>
+          <t>AuraSkypoolDXB-204</t>
         </is>
       </c>
       <c r="C205" t="n">
@@ -6596,7 +6596,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img205.png</t>
+          <t>AuraSkypoolDXB-205</t>
         </is>
       </c>
       <c r="C206" t="n">
@@ -6626,7 +6626,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img206.png</t>
+          <t>AuraSkypoolDXB-206</t>
         </is>
       </c>
       <c r="C207" t="n">
@@ -6656,7 +6656,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img207.png</t>
+          <t>AuraSkypoolDXB-207</t>
         </is>
       </c>
       <c r="C208" t="n">
@@ -6686,7 +6686,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img208.png</t>
+          <t>AuraSkypoolDXB-208</t>
         </is>
       </c>
       <c r="C209" t="n">
@@ -6716,7 +6716,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img209.png</t>
+          <t>AuraSkypoolDXB-209</t>
         </is>
       </c>
       <c r="C210" t="n">
@@ -6746,7 +6746,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img210.png</t>
+          <t>AuraSkypoolDXB-210</t>
         </is>
       </c>
       <c r="C211" t="n">
@@ -6776,7 +6776,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img211.png</t>
+          <t>AuraSkypoolDXB-211</t>
         </is>
       </c>
       <c r="C212" t="n">
@@ -6806,7 +6806,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>AuraSkypoolDXB-img212.png</t>
+          <t>AuraSkypoolDXB-212</t>
         </is>
       </c>
       <c r="C213" t="n">

</xml_diff>